<commit_message>
Scrum updated needs tasks :joy:
</commit_message>
<xml_diff>
--- a/Excel scrum.xlsx
+++ b/Excel scrum.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KYLU\Documents\GitHub\SEP4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDFCEEE-72F9-4504-A80A-6338914BDC61}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B37C3FC1-F4E0-4816-9FDF-8B48E3586CA6}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,13 +20,14 @@
     <sheet name="Sprint 4" sheetId="5" r:id="rId5"/>
     <sheet name="Sprint 5" sheetId="6" r:id="rId6"/>
     <sheet name="Sprint 6" sheetId="7" r:id="rId7"/>
+    <sheet name="Sprint 7" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="42">
   <si>
     <t>SPRINT 1</t>
   </si>
@@ -113,12 +114,6 @@
   </si>
   <si>
     <t>Match flight with weather data</t>
-  </si>
-  <si>
-    <t>Calculate average of thermal location considering the weather</t>
-  </si>
-  <si>
-    <t>As a user, I want to know the possible thermal locations</t>
   </si>
   <si>
     <t>Present the data in form of map</t>
@@ -425,70 +420,70 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>122</c:v>
+                  <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>116.45454545454545</c:v>
+                  <c:v>102.13636363636364</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>110.90909090909091</c:v>
+                  <c:v>97.27272727272728</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>105.36363636363636</c:v>
+                  <c:v>92.409090909090907</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>99.818181818181813</c:v>
+                  <c:v>87.545454545454547</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>94.272727272727266</c:v>
+                  <c:v>82.681818181818187</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>88.72727272727272</c:v>
+                  <c:v>77.818181818181813</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>83.181818181818187</c:v>
+                  <c:v>72.954545454545453</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>77.636363636363626</c:v>
+                  <c:v>68.090909090909093</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>72.090909090909093</c:v>
+                  <c:v>63.227272727272734</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>66.545454545454533</c:v>
+                  <c:v>58.363636363636367</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>60.999999999999993</c:v>
+                  <c:v>53.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>55.454545454545453</c:v>
+                  <c:v>48.63636363636364</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>49.909090909090907</c:v>
+                  <c:v>43.77272727272728</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>44.36363636363636</c:v>
+                  <c:v>38.909090909090907</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>38.818181818181813</c:v>
+                  <c:v>34.045454545454547</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>33.272727272727266</c:v>
+                  <c:v>29.181818181818187</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>27.72727272727272</c:v>
+                  <c:v>24.318181818181827</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>22.181818181818173</c:v>
+                  <c:v>19.454545454545467</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>16.636363636363626</c:v>
+                  <c:v>14.590909090909093</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>11.090909090909079</c:v>
+                  <c:v>9.7272727272727337</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>5.5454545454545325</c:v>
+                  <c:v>4.863636363636374</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -597,70 +592,70 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>122</c:v>
+                  <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>122</c:v>
+                  <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>122</c:v>
+                  <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>122</c:v>
+                  <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>122</c:v>
+                  <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>122</c:v>
+                  <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>122</c:v>
+                  <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>122</c:v>
+                  <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>122</c:v>
+                  <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>122</c:v>
+                  <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>122</c:v>
+                  <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>122</c:v>
+                  <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>122</c:v>
+                  <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>122</c:v>
+                  <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>122</c:v>
+                  <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>122</c:v>
+                  <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>122</c:v>
+                  <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>122</c:v>
+                  <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>122</c:v>
+                  <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>122</c:v>
+                  <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>122</c:v>
+                  <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>122</c:v>
+                  <c:v>107</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1738,8 +1733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1775,7 +1770,7 @@
       </c>
       <c r="F2">
         <f>SUM(D3:D14)</f>
-        <v>122</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1796,7 +1791,7 @@
       </c>
       <c r="F3">
         <f>F2/(COUNT(F17:F38))</f>
-        <v>5.5454545454545459</v>
+        <v>4.8636363636363633</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1876,7 +1871,7 @@
         <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -1893,10 +1888,10 @@
         <v>30</v>
       </c>
       <c r="C9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D9">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1907,23 +1902,9 @@
         <v>32</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
         <v>20</v>
       </c>
     </row>
@@ -1939,11 +1920,11 @@
       </c>
       <c r="G17">
         <f t="shared" ref="G17:G38" si="0">$F$2-(DATEDIF($F$17,F17,"D")*$F$3)</f>
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="H17">
         <f>F2</f>
-        <v>122</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
@@ -1953,11 +1934,11 @@
       </c>
       <c r="G18">
         <f t="shared" si="0"/>
-        <v>116.45454545454545</v>
+        <v>102.13636363636364</v>
       </c>
       <c r="H18">
         <f t="shared" ref="H18:H19" si="1">H17</f>
-        <v>122</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
@@ -1967,11 +1948,11 @@
       </c>
       <c r="G19">
         <f t="shared" si="0"/>
-        <v>110.90909090909091</v>
+        <v>97.27272727272728</v>
       </c>
       <c r="H19">
         <f t="shared" si="1"/>
-        <v>122</v>
+        <v>107</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
@@ -1981,11 +1962,11 @@
       </c>
       <c r="G20">
         <f t="shared" si="0"/>
-        <v>105.36363636363636</v>
+        <v>92.409090909090907</v>
       </c>
       <c r="H20">
         <f>H19</f>
-        <v>122</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1995,11 +1976,11 @@
       </c>
       <c r="G21">
         <f t="shared" si="0"/>
-        <v>99.818181818181813</v>
+        <v>87.545454545454547</v>
       </c>
       <c r="H21">
         <f t="shared" ref="H21:H38" si="2">H20</f>
-        <v>122</v>
+        <v>107</v>
       </c>
     </row>
     <row r="22" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2009,59 +1990,57 @@
       </c>
       <c r="G22">
         <f t="shared" si="0"/>
-        <v>94.272727272727266</v>
+        <v>82.681818181818187</v>
       </c>
       <c r="H22">
         <f t="shared" si="2"/>
-        <v>122</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="5" t="s">
-        <v>30</v>
-      </c>
+      <c r="B23" s="5"/>
       <c r="F23" s="6">
         <v>43244</v>
       </c>
       <c r="G23">
         <f t="shared" si="0"/>
-        <v>88.72727272727272</v>
+        <v>77.818181818181813</v>
       </c>
       <c r="H23">
         <f t="shared" si="2"/>
-        <v>122</v>
+        <v>107</v>
       </c>
     </row>
     <row r="24" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F24" s="6">
         <v>43245</v>
       </c>
       <c r="G24">
         <f t="shared" si="0"/>
-        <v>83.181818181818187</v>
+        <v>72.954545454545453</v>
       </c>
       <c r="H24">
         <f t="shared" si="2"/>
-        <v>122</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F25" s="6">
         <v>43246</v>
       </c>
       <c r="G25">
         <f t="shared" si="0"/>
-        <v>77.636363636363626</v>
+        <v>68.090909090909093</v>
       </c>
       <c r="H25">
         <f t="shared" si="2"/>
-        <v>122</v>
+        <v>107</v>
       </c>
     </row>
     <row r="26" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2070,11 +2049,11 @@
       </c>
       <c r="G26">
         <f t="shared" si="0"/>
-        <v>72.090909090909093</v>
+        <v>63.227272727272734</v>
       </c>
       <c r="H26">
         <f>H25</f>
-        <v>122</v>
+        <v>107</v>
       </c>
     </row>
     <row r="27" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2083,11 +2062,11 @@
       </c>
       <c r="G27">
         <f t="shared" si="0"/>
-        <v>66.545454545454533</v>
+        <v>58.363636363636367</v>
       </c>
       <c r="H27">
         <f t="shared" si="2"/>
-        <v>122</v>
+        <v>107</v>
       </c>
     </row>
     <row r="28" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2096,11 +2075,11 @@
       </c>
       <c r="G28">
         <f t="shared" si="0"/>
-        <v>60.999999999999993</v>
+        <v>53.5</v>
       </c>
       <c r="H28">
         <f t="shared" si="2"/>
-        <v>122</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2109,11 +2088,11 @@
       </c>
       <c r="G29">
         <f t="shared" si="0"/>
-        <v>55.454545454545453</v>
+        <v>48.63636363636364</v>
       </c>
       <c r="H29">
         <f t="shared" si="2"/>
-        <v>122</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2122,11 +2101,11 @@
       </c>
       <c r="G30">
         <f t="shared" si="0"/>
-        <v>49.909090909090907</v>
+        <v>43.77272727272728</v>
       </c>
       <c r="H30">
         <f t="shared" si="2"/>
-        <v>122</v>
+        <v>107</v>
       </c>
     </row>
     <row r="31" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2135,11 +2114,11 @@
       </c>
       <c r="G31">
         <f t="shared" si="0"/>
-        <v>44.36363636363636</v>
+        <v>38.909090909090907</v>
       </c>
       <c r="H31">
         <f t="shared" si="2"/>
-        <v>122</v>
+        <v>107</v>
       </c>
     </row>
     <row r="32" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2148,11 +2127,11 @@
       </c>
       <c r="G32">
         <f t="shared" si="0"/>
-        <v>38.818181818181813</v>
+        <v>34.045454545454547</v>
       </c>
       <c r="H32">
         <f t="shared" si="2"/>
-        <v>122</v>
+        <v>107</v>
       </c>
     </row>
     <row r="33" spans="6:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2161,11 +2140,11 @@
       </c>
       <c r="G33">
         <f t="shared" si="0"/>
-        <v>33.272727272727266</v>
+        <v>29.181818181818187</v>
       </c>
       <c r="H33">
         <f t="shared" si="2"/>
-        <v>122</v>
+        <v>107</v>
       </c>
     </row>
     <row r="34" spans="6:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2174,11 +2153,11 @@
       </c>
       <c r="G34">
         <f t="shared" si="0"/>
-        <v>27.72727272727272</v>
+        <v>24.318181818181827</v>
       </c>
       <c r="H34">
         <f t="shared" si="2"/>
-        <v>122</v>
+        <v>107</v>
       </c>
     </row>
     <row r="35" spans="6:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2187,11 +2166,11 @@
       </c>
       <c r="G35">
         <f t="shared" si="0"/>
-        <v>22.181818181818173</v>
+        <v>19.454545454545467</v>
       </c>
       <c r="H35">
         <f t="shared" si="2"/>
-        <v>122</v>
+        <v>107</v>
       </c>
     </row>
     <row r="36" spans="6:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2200,11 +2179,11 @@
       </c>
       <c r="G36">
         <f t="shared" si="0"/>
-        <v>16.636363636363626</v>
+        <v>14.590909090909093</v>
       </c>
       <c r="H36">
         <f t="shared" si="2"/>
-        <v>122</v>
+        <v>107</v>
       </c>
     </row>
     <row r="37" spans="6:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2213,11 +2192,11 @@
       </c>
       <c r="G37">
         <f t="shared" si="0"/>
-        <v>11.090909090909079</v>
+        <v>9.7272727272727337</v>
       </c>
       <c r="H37">
         <f t="shared" si="2"/>
-        <v>122</v>
+        <v>107</v>
       </c>
     </row>
     <row r="38" spans="6:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2226,11 +2205,11 @@
       </c>
       <c r="G38">
         <f t="shared" si="0"/>
-        <v>5.5454545454545325</v>
+        <v>4.863636363636374</v>
       </c>
       <c r="H38">
         <f t="shared" si="2"/>
-        <v>122</v>
+        <v>107</v>
       </c>
     </row>
     <row r="39" spans="6:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -4345,7 +4324,7 @@
         <v>43241</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>14</v>
@@ -4360,7 +4339,7 @@
         <v>As a administrator, I want to see the converted weather files in the database</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
@@ -4371,7 +4350,7 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>4</v>
@@ -4379,10 +4358,10 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C8" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -5428,7 +5407,7 @@
         <v>43244</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>14</v>
@@ -5462,7 +5441,7 @@
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D7" s="8" t="s">
         <v>4</v>
@@ -5470,7 +5449,7 @@
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C8" s="8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>4</v>
@@ -6501,7 +6480,7 @@
         <v>43247</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>14</v>
@@ -7544,7 +7523,7 @@
         <v>43250</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>14</v>
@@ -7570,7 +7549,7 @@
         <v>22</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -8569,7 +8548,7 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8578,12 +8557,12 @@
   <dimension ref="A2:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.42578125" customWidth="1"/>
     <col min="3" max="3" width="97.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8592,7 +8571,7 @@
         <v>43253</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>14</v>
@@ -8618,7 +8597,7 @@
         <v>22</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>38</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -8638,4 +8617,48 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54FC9DD3-863D-4AD0-AFE9-B5CE848E682A}">
+  <dimension ref="A2:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
+        <v>43256</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C3" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C4" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>